<commit_message>
Update Excel files: modified bioyond_cell and material_template with new data
</commit_message>
<xml_diff>
--- a/unilabos/devices/workstation/bioyond_studio/bioyond_cell/material_template.xlsx
+++ b/unilabos/devices/workstation/bioyond_studio/bioyond_cell/material_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24960" windowHeight="14020"/>
+    <workbookView windowWidth="24980" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="入库" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>LiFSI</t>
+    <t>LiPF6</t>
   </si>
   <si>
     <t>8</t>
@@ -1142,8 +1142,8 @@
   <sheetPr/>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="17.6"/>
@@ -1758,7 +1758,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I1 A2:E2 G2:I2 A3:I14 A15:E16 A17:I25 A26:E26 G26:I26 A27:E28 G27:I28 A29:I40" numberStoredAsText="1"/>
+    <ignoredError sqref="A29:I40 G26:I28 A26:E28 A17:I25 A15:E16 A3:I14 G2:I2 A2:E2 A1:I1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>